<commit_message>
added i know it feature
</commit_message>
<xml_diff>
--- a/data/drbc-deck-1.xlsx
+++ b/data/drbc-deck-1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tylerbradley/Documents/shiny-flash-cards/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A2AAABE-8258-B74B-8B0F-F603FB3DF998}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2E46D0C-2E6C-8A4B-A49E-A1EE86A1B4FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16920" yWindow="0" windowWidth="16680" windowHeight="21000" xr2:uid="{DFD306EA-B649-A841-BEF9-F74566FD3957}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{DFD306EA-B649-A841-BEF9-F74566FD3957}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="218">
   <si>
     <t>Question</t>
   </si>
@@ -660,6 +660,33 @@
   </si>
   <si>
     <t>Equitable Allocation</t>
+  </si>
+  <si>
+    <t>FFMP</t>
+  </si>
+  <si>
+    <t>Flexible Flow Management Plan</t>
+  </si>
+  <si>
+    <t>Address: Water Supply, Instream Flow Needs, and Spill Migration</t>
+  </si>
+  <si>
+    <t>Based on Reservoir Releases</t>
+  </si>
+  <si>
+    <t>Renewal of FFMP requires unanimous vote from PA, NJ, NY, DE, and NYC</t>
+  </si>
+  <si>
+    <t>Flow Management</t>
+  </si>
+  <si>
+    <t>Non-drought Flow Targets</t>
+  </si>
+  <si>
+    <t>Montague - 1750 cfs (1130 MGD)</t>
+  </si>
+  <si>
+    <t>Trenton - 3000 cfs (1940 MGD)</t>
   </si>
 </sst>
 </file>
@@ -1016,10 +1043,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FC9D4D1-F6A9-C940-A3C3-6AD155BF6F59}">
-  <dimension ref="A1:C154"/>
+  <dimension ref="A1:C160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A122" zoomScale="85" workbookViewId="0">
-      <selection activeCell="A155" sqref="A155"/>
+    <sheetView tabSelected="1" topLeftCell="A137" zoomScale="85" workbookViewId="0">
+      <selection activeCell="D161" sqref="D161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="112.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2235,6 +2262,9 @@
       <c r="B110" s="1" t="s">
         <v>153</v>
       </c>
+      <c r="C110" s="1" t="s">
+        <v>214</v>
+      </c>
     </row>
     <row r="111" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
@@ -2243,6 +2273,9 @@
       <c r="B111" s="1" t="s">
         <v>155</v>
       </c>
+      <c r="C111" s="1" t="s">
+        <v>214</v>
+      </c>
     </row>
     <row r="112" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
@@ -2251,341 +2284,530 @@
       <c r="B112" s="1" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="113" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="C112" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>154</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="114" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="C113" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
         <v>158</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="115" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="C114" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
         <v>158</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="116" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="C115" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
         <v>158</v>
       </c>
       <c r="B116" s="1" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="117" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="C116" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
         <v>158</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="118" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="C117" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
         <v>158</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="119" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="C118" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
         <v>164</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="120" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="C119" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>164</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="121" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="C120" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
         <v>164</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="122" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="C121" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
         <v>164</v>
       </c>
       <c r="B122" s="1" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="123" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="C122" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
         <v>169</v>
       </c>
       <c r="B123" s="1" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="124" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="C123" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
         <v>171</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="125" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="C124" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>171</v>
       </c>
       <c r="B125" s="1" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="126" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="C125" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
         <v>171</v>
       </c>
       <c r="B126" s="1" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="127" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="C126" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
         <v>175</v>
       </c>
       <c r="B127" s="1" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="128" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="C127" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
         <v>175</v>
       </c>
       <c r="B128" s="1" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="129" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="C128" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
         <v>175</v>
       </c>
       <c r="B129" s="1" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="130" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="C129" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
         <v>179</v>
       </c>
       <c r="B130" s="1" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="131" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="C130" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
         <v>179</v>
       </c>
       <c r="B131" s="1" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="132" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="C131" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
         <v>179</v>
       </c>
       <c r="B132" s="1" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="133" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="C132" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
         <v>179</v>
       </c>
       <c r="B133" s="1" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="134" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="C133" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
         <v>179</v>
       </c>
       <c r="B134" s="1" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="135" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="C134" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
         <v>179</v>
       </c>
       <c r="B135" s="1" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="136" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="C135" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
         <v>186</v>
       </c>
       <c r="B136" s="1" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="137" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="C136" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
         <v>186</v>
       </c>
       <c r="B137" s="1" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="138" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="C137" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
         <v>186</v>
       </c>
       <c r="B138" s="1" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="139" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="C138" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
         <v>186</v>
       </c>
       <c r="B139" s="1" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="140" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="C139" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
         <v>186</v>
       </c>
       <c r="B140" s="1" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="141" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="C140" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
         <v>179</v>
       </c>
       <c r="B141" s="1" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="142" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="C141" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
         <v>179</v>
       </c>
       <c r="B142" s="1" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="143" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="C142" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
         <v>179</v>
       </c>
       <c r="B143" s="1" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="144" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="C143" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
         <v>179</v>
       </c>
       <c r="B144" s="1" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="145" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="C144" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
         <v>196</v>
       </c>
       <c r="B145" s="1" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="146" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="C145" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
         <v>196</v>
       </c>
       <c r="B146" s="1" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="147" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="C146" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
         <v>196</v>
       </c>
       <c r="B147" s="1" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="148" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="C147" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
         <v>196</v>
       </c>
       <c r="B148" s="1" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="149" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="C148" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
         <v>201</v>
       </c>
       <c r="B149" s="1" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="150" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="C149" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
         <v>201</v>
       </c>
       <c r="B150" s="1" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="151" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="C150" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
         <v>204</v>
       </c>
       <c r="B151" s="1" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="152" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="C151" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
         <v>204</v>
       </c>
       <c r="B152" s="1" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="153" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="C152" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
         <v>204</v>
       </c>
       <c r="B153" s="1" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="154" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="C153" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
         <v>204</v>
       </c>
       <c r="B154" s="1" t="s">
         <v>208</v>
+      </c>
+      <c r="C154" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A155" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="C155" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A156" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C156" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A157" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C157" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A158" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C158" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A159" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A160" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>217</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating how button clicks effect the card
</commit_message>
<xml_diff>
--- a/data/drbc-deck-1.xlsx
+++ b/data/drbc-deck-1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tylerbradley/Documents/shiny-flash-cards/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E910DEA-EAFB-C34E-8B0A-B3D8197BF6C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74442C9F-9988-A44E-ACD8-7E60966E5C2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16920" yWindow="0" windowWidth="16680" windowHeight="21000" xr2:uid="{DFD306EA-B649-A841-BEF9-F74566FD3957}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{DFD306EA-B649-A841-BEF9-F74566FD3957}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="301">
   <si>
     <t>Question</t>
   </si>
@@ -425,9 +425,6 @@
     <t>Should internal groups write the plan or is there time to engage external stakeholders</t>
   </si>
   <si>
-    <t>Determining who decides the priorotes</t>
-  </si>
-  <si>
     <t>Water Characteristics</t>
   </si>
   <si>
@@ -936,6 +933,9 @@
   </si>
   <si>
     <t>DRWI</t>
+  </si>
+  <si>
+    <t>Determining who decides the priorites</t>
   </si>
 </sst>
 </file>
@@ -1300,8 +1300,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FC9D4D1-F6A9-C940-A3C3-6AD155BF6F59}">
   <dimension ref="A1:C224"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A183" zoomScale="85" workbookViewId="0">
-      <selection activeCell="D221" sqref="D221"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="125" workbookViewId="0">
+      <selection activeCell="B96" sqref="B96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="112.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2166,7 +2166,7 @@
         <v>84</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -2177,7 +2177,7 @@
         <v>85</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2188,7 +2188,7 @@
         <v>111</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -2199,7 +2199,7 @@
         <v>112</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -2210,7 +2210,7 @@
         <v>113</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2221,7 +2221,7 @@
         <v>114</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2232,7 +2232,7 @@
         <v>116</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2243,7 +2243,7 @@
         <v>117</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2254,7 +2254,7 @@
         <v>118</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2265,7 +2265,7 @@
         <v>119</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2276,7 +2276,7 @@
         <v>120</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2287,7 +2287,7 @@
         <v>121</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2298,7 +2298,7 @@
         <v>123</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -2309,7 +2309,7 @@
         <v>124</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2320,7 +2320,7 @@
         <v>126</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2331,7 +2331,7 @@
         <v>127</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2342,7 +2342,7 @@
         <v>128</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -2353,7 +2353,7 @@
         <v>129</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2361,1415 +2361,1418 @@
         <v>125</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>130</v>
+        <v>300</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B97" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B97" s="1" t="s">
-        <v>132</v>
-      </c>
       <c r="C97" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B102" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B102" s="1" t="s">
-        <v>138</v>
-      </c>
       <c r="C102" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B103" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B103" s="1" t="s">
-        <v>140</v>
-      </c>
       <c r="C103" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B104" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B104" s="1" t="s">
-        <v>142</v>
-      </c>
       <c r="C104" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B106" s="2">
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B107" s="3">
         <v>0.05</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C108" s="1" t="s">
         <v>150</v>
-      </c>
-      <c r="B108" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="C108" s="1" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B109" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B109" s="1" t="s">
-        <v>149</v>
-      </c>
       <c r="C109" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B110" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="B110" s="1" t="s">
-        <v>153</v>
-      </c>
       <c r="C110" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B111" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="B111" s="1" t="s">
-        <v>155</v>
-      </c>
       <c r="C111" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B114" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="B114" s="1" t="s">
-        <v>159</v>
-      </c>
       <c r="C114" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="116" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B119" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="B119" s="1" t="s">
-        <v>165</v>
-      </c>
       <c r="C119" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="123" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B123" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="B123" s="1" t="s">
-        <v>170</v>
-      </c>
       <c r="C123" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="124" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B124" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="B124" s="1" t="s">
-        <v>172</v>
-      </c>
       <c r="C124" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="127" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B127" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="B127" s="1" t="s">
-        <v>176</v>
-      </c>
       <c r="C127" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="128" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="129" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="130" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B130" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="B130" s="1" t="s">
-        <v>180</v>
-      </c>
       <c r="C130" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="131" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="132" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="133" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="134" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="135" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="136" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B136" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B136" s="1" t="s">
-        <v>187</v>
-      </c>
       <c r="C136" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="137" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="138" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="139" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="140" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="141" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="142" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="143" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="144" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="145" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B145" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="B145" s="1" t="s">
-        <v>197</v>
-      </c>
       <c r="C145" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="146" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="147" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="148" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="149" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B149" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="B149" s="1" t="s">
-        <v>202</v>
-      </c>
       <c r="C149" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="150" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="151" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B151" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="B151" s="1" t="s">
-        <v>205</v>
-      </c>
       <c r="C151" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="152" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="153" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="154" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="155" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B155" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="B155" s="1" t="s">
-        <v>210</v>
-      </c>
       <c r="C155" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="156" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="157" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="158" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="159" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B159" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="B159" s="1" t="s">
-        <v>216</v>
-      </c>
       <c r="C159" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="160" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="161" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B161" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="B161" s="1" t="s">
-        <v>219</v>
-      </c>
       <c r="C161" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="162" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B162" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="B162" s="1" t="s">
-        <v>221</v>
-      </c>
       <c r="C162" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="163" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B163" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="B163" s="1" t="s">
-        <v>223</v>
-      </c>
       <c r="C163" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="164" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B164" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="B164" s="1" t="s">
-        <v>225</v>
-      </c>
       <c r="C164" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="165" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B165" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="B165" s="1" t="s">
-        <v>227</v>
-      </c>
       <c r="C165" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="166" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="167" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="168" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="169" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="170" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="171" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="172" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B172" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="B172" s="1" t="s">
-        <v>235</v>
-      </c>
       <c r="C172" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="173" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A173" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B173" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="B173" s="1" t="s">
-        <v>237</v>
-      </c>
       <c r="C173" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="174" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="175" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A175" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="176" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="177" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A177" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="178" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="179" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B179" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="B179" s="1" t="s">
-        <v>245</v>
-      </c>
       <c r="C179" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="180" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A180" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="181" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A181" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="182" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A182" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="183" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A183" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="B183" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="B183" s="1" t="s">
-        <v>250</v>
-      </c>
       <c r="C183" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="184" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A184" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="185" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A185" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="186" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A186" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="187" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A187" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="188" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A188" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="B188" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="B188" s="1" t="s">
-        <v>256</v>
-      </c>
       <c r="C188" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="189" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A189" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C189" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="190" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A190" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="191" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A191" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="192" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A192" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="B192" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="B192" s="1" t="s">
-        <v>261</v>
-      </c>
       <c r="C192" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="193" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A193" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C193" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="194" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A194" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C194" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="195" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A195" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C195" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="196" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A196" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C196" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="197" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A197" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C197" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="198" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A198" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C198" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="199" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A199" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B199" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="B199" s="1" t="s">
-        <v>269</v>
-      </c>
       <c r="C199" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="200" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A200" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C200" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="201" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A201" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C201" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="202" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A202" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C202" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="203" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A203" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C203" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="204" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A204" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C204" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="205" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A205" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B205" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="B205" s="1" t="s">
-        <v>276</v>
-      </c>
       <c r="C205" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="206" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A206" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C206" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="207" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A207" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C207" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="208" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A208" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="B208" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="B208" s="1" t="s">
-        <v>280</v>
-      </c>
       <c r="C208" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="209" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A209" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C209" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="210" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A210" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C210" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="211" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A211" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C211" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="212" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A212" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C212" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="213" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A213" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C213" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="214" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A214" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="B214" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="B214" s="1" t="s">
-        <v>286</v>
-      </c>
       <c r="C214" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="215" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A215" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C215" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="216" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A216" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C216" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="217" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A217" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C217" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="218" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A218" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="B218" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="B218" s="1" t="s">
+      <c r="C218" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A219" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="B219" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="C218" s="1" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="219" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="B219" s="1" t="s">
-        <v>292</v>
-      </c>
       <c r="C219" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="220" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A220" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="B220" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="B220" s="1" t="s">
-        <v>294</v>
-      </c>
       <c r="C220" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="221" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A221" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C221" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="222" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A222" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="B222" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="B222" s="1" t="s">
-        <v>297</v>
-      </c>
       <c r="C222" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="223" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A223" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C223" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="224" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A224" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C224" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
   </sheetData>

</xml_diff>